<commit_message>
done changes for MZ region
</commit_message>
<xml_diff>
--- a/src/global/utils/file-utils/locators(2).xlsx
+++ b/src/global/utils/file-utils/locators(2).xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="14"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="HomePage"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2672" uniqueCount="762">
   <si>
     <t>page</t>
   </si>
@@ -1789,6 +1789,9 @@
   </si>
   <si>
     <t>Betting Rules</t>
+  </si>
+  <si>
+    <t>bettingRulesMZ</t>
   </si>
   <si>
     <t>bettingRules</t>
@@ -2537,9 +2540,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2575,6 +2575,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2947,10 +2950,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>8</v>
@@ -2958,8 +2961,8 @@
       <c r="D2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>727</v>
+      <c r="E2" s="29" t="s">
+        <v>728</v>
       </c>
       <c r="F2" s="8">
         <v>1</v>
@@ -2967,10 +2970,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>8</v>
@@ -2978,35 +2981,35 @@
       <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>729</v>
+      <c r="E3" s="29" t="s">
+        <v>730</v>
       </c>
       <c r="F3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="E4" s="30" t="s">
+        <v>732</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>8</v>
@@ -3014,17 +3017,17 @@
       <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>733</v>
+      <c r="E5" s="29" t="s">
+        <v>734</v>
       </c>
       <c r="F5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -3032,17 +3035,17 @@
       <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>735</v>
+      <c r="E6" s="29" t="s">
+        <v>736</v>
       </c>
       <c r="F6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>8</v>
@@ -3050,71 +3053,71 @@
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="30" t="s">
-        <v>737</v>
+      <c r="E7" s="29" t="s">
+        <v>738</v>
       </c>
       <c r="F7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>739</v>
-      </c>
-      <c r="E8" s="30" t="s">
+        <v>740</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>741</v>
-      </c>
-      <c r="E9" s="30" t="s">
+        <v>742</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>743</v>
-      </c>
-      <c r="E10" s="30" t="s">
+        <v>744</v>
+      </c>
+      <c r="E10" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>8</v>
@@ -3122,151 +3125,151 @@
       <c r="D11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>745</v>
+      <c r="E11" s="29" t="s">
+        <v>746</v>
       </c>
       <c r="F11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>747</v>
-      </c>
-      <c r="E12" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>748</v>
-      </c>
-      <c r="E13" s="30" t="s">
+        <v>749</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>750</v>
-      </c>
-      <c r="E14" s="30" t="s">
+        <v>751</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>752</v>
-      </c>
-      <c r="E15" s="30" t="s">
+        <v>753</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>754</v>
-      </c>
-      <c r="E16" s="30" t="s">
+        <v>755</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>756</v>
-      </c>
-      <c r="E17" s="30" t="s">
+        <v>757</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>758</v>
-      </c>
-      <c r="E18" s="30" t="s">
+        <v>759</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>760</v>
-      </c>
-      <c r="E19" s="30" t="s">
+        <v>761</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="8"/>
@@ -3276,7 +3279,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="30"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -3284,7 +3287,7 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="30"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -3292,7 +3295,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="30"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
@@ -3300,7 +3303,7 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="30"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
@@ -3308,7 +3311,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="30"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -3316,7 +3319,7 @@
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="30"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
@@ -3324,7 +3327,7 @@
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="30"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -3332,7 +3335,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="30"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
@@ -3340,7 +3343,7 @@
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="30"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
@@ -3348,7 +3351,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="30"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -3356,7 +3359,7 @@
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="30"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -3364,7 +3367,7 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="30"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
@@ -3372,7 +3375,7 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="30"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
@@ -3380,7 +3383,7 @@
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="30"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
@@ -3388,7 +3391,7 @@
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="30"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
@@ -3396,7 +3399,7 @@
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="30"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
@@ -3404,7 +3407,7 @@
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="30"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
@@ -3412,7 +3415,7 @@
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="30"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
@@ -3420,7 +3423,7 @@
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="30"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
@@ -3428,7 +3431,7 @@
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="30"/>
+      <c r="E39" s="29"/>
       <c r="F39" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -3436,7 +3439,7 @@
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="30"/>
+      <c r="E40" s="29"/>
       <c r="F40" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
@@ -3444,7 +3447,7 @@
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="30"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
@@ -3452,7 +3455,7 @@
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="30"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
@@ -3460,7 +3463,7 @@
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="30"/>
+      <c r="E43" s="29"/>
       <c r="F43" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
@@ -3468,7 +3471,7 @@
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="30"/>
+      <c r="E44" s="29"/>
       <c r="F44" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
@@ -3476,7 +3479,7 @@
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="30"/>
+      <c r="E45" s="29"/>
       <c r="F45" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -3484,7 +3487,7 @@
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="30"/>
+      <c r="E46" s="29"/>
       <c r="F46" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
@@ -3492,7 +3495,7 @@
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="30"/>
+      <c r="E47" s="29"/>
       <c r="F47" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -3500,7 +3503,7 @@
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="30"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -3508,7 +3511,7 @@
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="30"/>
+      <c r="E49" s="29"/>
       <c r="F49" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -3517,7 +3520,7 @@
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
-      <c r="F50" s="22"/>
+      <c r="F50" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="14"/>
@@ -3525,7 +3528,7 @@
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
-      <c r="F51" s="22"/>
+      <c r="F51" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="14"/>
@@ -3533,7 +3536,7 @@
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
-      <c r="F52" s="22"/>
+      <c r="F52" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="14"/>
@@ -3541,7 +3544,7 @@
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
-      <c r="F53" s="22"/>
+      <c r="F53" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="14"/>
@@ -3549,7 +3552,7 @@
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
-      <c r="F54" s="22"/>
+      <c r="F54" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="14"/>
@@ -3565,7 +3568,7 @@
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
-      <c r="F56" s="22"/>
+      <c r="F56" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="14"/>
@@ -3573,7 +3576,7 @@
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
-      <c r="F57" s="22"/>
+      <c r="F57" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="14"/>
@@ -3597,7 +3600,7 @@
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
-      <c r="F60" s="22"/>
+      <c r="F60" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="14"/>
@@ -3605,7 +3608,7 @@
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
-      <c r="F61" s="22"/>
+      <c r="F61" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="14"/>
@@ -3613,7 +3616,7 @@
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
-      <c r="F62" s="22"/>
+      <c r="F62" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="14"/>
@@ -3621,7 +3624,7 @@
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
-      <c r="F63" s="22"/>
+      <c r="F63" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="14"/>
@@ -3636,7 +3639,7 @@
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
-      <c r="E65" s="30"/>
+      <c r="E65" s="29"/>
       <c r="F65" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
@@ -3645,7 +3648,7 @@
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
-      <c r="F66" s="22"/>
+      <c r="F66" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="14"/>
@@ -3653,7 +3656,7 @@
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
-      <c r="F67" s="22"/>
+      <c r="F67" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="14"/>
@@ -3661,7 +3664,7 @@
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
-      <c r="F68" s="22"/>
+      <c r="F68" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="14"/>
@@ -3669,7 +3672,7 @@
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
-      <c r="F69" s="22"/>
+      <c r="F69" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="14"/>
@@ -3677,7 +3680,7 @@
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
-      <c r="F70" s="22"/>
+      <c r="F70" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="14"/>
@@ -3685,7 +3688,7 @@
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
-      <c r="F71" s="22"/>
+      <c r="F71" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="14"/>
@@ -3693,7 +3696,7 @@
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
-      <c r="F72" s="22"/>
+      <c r="F72" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="14"/>
@@ -3701,7 +3704,7 @@
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
-      <c r="F73" s="22"/>
+      <c r="F73" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="14"/>
@@ -3717,7 +3720,7 @@
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
-      <c r="F75" s="22"/>
+      <c r="F75" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="14"/>
@@ -3725,7 +3728,7 @@
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
-      <c r="F76" s="22"/>
+      <c r="F76" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="14"/>
@@ -3741,7 +3744,7 @@
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
-      <c r="F78" s="22"/>
+      <c r="F78" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="14"/>
@@ -3757,7 +3760,7 @@
       <c r="C80" s="14"/>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
-      <c r="F80" s="22"/>
+      <c r="F80" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="14"/>
@@ -3765,7 +3768,7 @@
       <c r="C81" s="14"/>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
-      <c r="F81" s="22"/>
+      <c r="F81" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="14"/>
@@ -3773,7 +3776,7 @@
       <c r="C82" s="14"/>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
-      <c r="F82" s="22"/>
+      <c r="F82" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="14"/>
@@ -3781,7 +3784,7 @@
       <c r="C83" s="14"/>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
-      <c r="F83" s="22"/>
+      <c r="F83" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="14"/>
@@ -3789,14 +3792,14 @@
       <c r="C84" s="14"/>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
-      <c r="F84" s="22"/>
+      <c r="F84" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="14"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
-      <c r="E85" s="30"/>
+      <c r="E85" s="29"/>
       <c r="F85" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -3804,7 +3807,7 @@
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
-      <c r="E86" s="30"/>
+      <c r="E86" s="29"/>
       <c r="F86" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -3812,7 +3815,7 @@
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
-      <c r="E87" s="30"/>
+      <c r="E87" s="29"/>
       <c r="F87" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -3820,7 +3823,7 @@
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
-      <c r="E88" s="30"/>
+      <c r="E88" s="29"/>
       <c r="F88" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
@@ -3828,7 +3831,7 @@
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
-      <c r="E89" s="30"/>
+      <c r="E89" s="29"/>
       <c r="F89" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
@@ -3836,7 +3839,7 @@
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
-      <c r="E90" s="30"/>
+      <c r="E90" s="29"/>
       <c r="F90" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
@@ -3844,7 +3847,7 @@
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
-      <c r="E91" s="30"/>
+      <c r="E91" s="29"/>
       <c r="F91" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
@@ -3852,7 +3855,7 @@
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
-      <c r="E92" s="30"/>
+      <c r="E92" s="29"/>
       <c r="F92" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
@@ -3860,7 +3863,7 @@
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
-      <c r="E93" s="30"/>
+      <c r="E93" s="29"/>
       <c r="F93" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
@@ -3868,7 +3871,7 @@
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
-      <c r="E94" s="30"/>
+      <c r="E94" s="29"/>
       <c r="F94" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
@@ -3876,7 +3879,7 @@
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
-      <c r="E95" s="30"/>
+      <c r="E95" s="29"/>
       <c r="F95" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
@@ -3884,7 +3887,7 @@
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
-      <c r="E96" s="30"/>
+      <c r="E96" s="29"/>
       <c r="F96" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
@@ -3892,7 +3895,7 @@
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
-      <c r="E97" s="30"/>
+      <c r="E97" s="29"/>
       <c r="F97" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -3900,7 +3903,7 @@
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
-      <c r="E98" s="30"/>
+      <c r="E98" s="29"/>
       <c r="F98" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
@@ -3908,7 +3911,7 @@
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
-      <c r="E99" s="30"/>
+      <c r="E99" s="29"/>
       <c r="F99" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
@@ -3916,7 +3919,7 @@
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
-      <c r="E100" s="30"/>
+      <c r="E100" s="29"/>
       <c r="F100" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
@@ -3924,7 +3927,7 @@
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
-      <c r="E101" s="30"/>
+      <c r="E101" s="29"/>
       <c r="F101" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
@@ -3932,7 +3935,7 @@
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
-      <c r="E102" s="30"/>
+      <c r="E102" s="29"/>
       <c r="F102" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
@@ -3940,7 +3943,7 @@
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
-      <c r="E103" s="30"/>
+      <c r="E103" s="29"/>
       <c r="F103" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
@@ -3948,7 +3951,7 @@
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
-      <c r="E104" s="30"/>
+      <c r="E104" s="29"/>
       <c r="F104" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
@@ -3956,7 +3959,7 @@
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
-      <c r="E105" s="30"/>
+      <c r="E105" s="29"/>
       <c r="F105" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
@@ -3964,7 +3967,7 @@
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
-      <c r="E106" s="30"/>
+      <c r="E106" s="29"/>
       <c r="F106" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
@@ -3972,7 +3975,7 @@
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
-      <c r="E107" s="30"/>
+      <c r="E107" s="29"/>
       <c r="F107" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
@@ -3980,7 +3983,7 @@
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
-      <c r="E108" s="30"/>
+      <c r="E108" s="29"/>
       <c r="F108" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
@@ -3989,7 +3992,7 @@
       <c r="C109" s="14"/>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
-      <c r="F109" s="22"/>
+      <c r="F109" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="6"/>
@@ -3997,7 +4000,7 @@
       <c r="C110" s="14"/>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
-      <c r="F110" s="22"/>
+      <c r="F110" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="6"/>
@@ -4005,7 +4008,7 @@
       <c r="C111" s="14"/>
       <c r="D111" s="14"/>
       <c r="E111" s="14"/>
-      <c r="F111" s="22"/>
+      <c r="F111" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="6"/>
@@ -4040,20 +4043,20 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="21"/>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="20"/>
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5028,7 +5031,7 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -5048,7 +5051,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -5068,7 +5071,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -5088,7 +5091,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -5108,7 +5111,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -5123,10 +5126,10 @@
       <c r="E5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -5146,7 +5149,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -5161,10 +5164,10 @@
       <c r="E7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -5179,10 +5182,10 @@
       <c r="E8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -5197,10 +5200,10 @@
       <c r="E9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -5215,10 +5218,10 @@
       <c r="E10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -5233,10 +5236,10 @@
       <c r="E11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="22"/>
+      <c r="F11" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -5251,10 +5254,10 @@
       <c r="E12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -5269,10 +5272,10 @@
       <c r="E13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B14" s="14" t="s">
@@ -5287,10 +5290,10 @@
       <c r="E14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -5305,10 +5308,10 @@
       <c r="E15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -5323,10 +5326,10 @@
       <c r="E16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -5341,10 +5344,10 @@
       <c r="E17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -5359,10 +5362,10 @@
       <c r="E18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -5382,7 +5385,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -5402,7 +5405,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -5422,7 +5425,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -5442,7 +5445,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -5462,7 +5465,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -5477,10 +5480,10 @@
       <c r="E24" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="22"/>
+      <c r="F24" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -5500,7 +5503,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B26" s="14" t="s">
@@ -5520,7 +5523,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B27" s="14" t="s">
@@ -5538,7 +5541,7 @@
       <c r="F27" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -5558,7 +5561,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B29" s="14" t="s">
@@ -5573,12 +5576,12 @@
       <c r="E29" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="21">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B30" s="14" t="s">
@@ -5593,10 +5596,10 @@
       <c r="E30" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="22"/>
+      <c r="F30" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B31" s="14" t="s">
@@ -5611,10 +5614,10 @@
       <c r="E31" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="22"/>
+      <c r="F31" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -5629,10 +5632,10 @@
       <c r="E32" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B33" s="14" t="s">
@@ -5652,7 +5655,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B34" s="14" t="s">
@@ -5672,7 +5675,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="20" t="s">
         <v>325</v>
       </c>
       <c r="B35" s="14" t="s">
@@ -5687,7 +5690,7 @@
       <c r="E35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="22"/>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6517,7 +6520,7 @@
       <c r="C30" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="17" t="s">
         <v>269</v>
       </c>
       <c r="E30" s="17" t="s">
@@ -6559,7 +6562,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9641,7 +9644,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>173</v>
@@ -9661,7 +9664,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>184</v>
@@ -9673,7 +9676,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F3" s="8">
         <v>0</v>
@@ -9681,7 +9684,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>186</v>
@@ -9701,7 +9704,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>188</v>
@@ -9721,7 +9724,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>190</v>
@@ -9741,7 +9744,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>192</v>
@@ -9761,7 +9764,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>194</v>
@@ -9773,7 +9776,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F8" s="8">
         <v>0</v>
@@ -9781,7 +9784,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>196</v>
@@ -9793,7 +9796,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F9" s="8">
         <v>0</v>
@@ -9801,7 +9804,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>198</v>
@@ -9813,7 +9816,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="F10" s="8">
         <v>0</v>
@@ -9821,7 +9824,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>200</v>
@@ -9833,7 +9836,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -9841,7 +9844,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>202</v>
@@ -9853,7 +9856,7 @@
         <v>30</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -9861,7 +9864,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>204</v>
@@ -9873,7 +9876,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -9881,7 +9884,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>206</v>
@@ -9901,7 +9904,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>208</v>
@@ -9913,7 +9916,7 @@
         <v>30</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -9921,7 +9924,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>210</v>
@@ -9933,7 +9936,7 @@
         <v>30</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
@@ -9941,7 +9944,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>212</v>
@@ -9953,7 +9956,7 @@
         <v>30</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F17" s="8">
         <v>0</v>
@@ -9961,7 +9964,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>214</v>
@@ -9981,7 +9984,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>381</v>
@@ -10001,7 +10004,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>217</v>
@@ -10021,7 +10024,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>218</v>
@@ -10041,7 +10044,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>32</v>
@@ -10061,7 +10064,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>220</v>
@@ -10081,7 +10084,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>222</v>
@@ -10101,7 +10104,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>224</v>
@@ -10121,7 +10124,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>226</v>
@@ -10221,7 +10224,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>23</v>
@@ -10272,13 +10275,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="14" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>23</v>
@@ -10289,13 +10292,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="14" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>23</v>
@@ -10304,13 +10307,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="14" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>23</v>
@@ -10319,13 +10322,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="14" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>23</v>
@@ -10334,13 +10337,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="14" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>23</v>
@@ -10355,7 +10358,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>23</v>
@@ -10364,13 +10367,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>23</v>
@@ -10379,13 +10382,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>23</v>
@@ -10394,13 +10397,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>23</v>
@@ -10409,7 +10412,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>8</v>
@@ -10418,7 +10421,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="E11" s="8"/>
     </row>
@@ -10490,7 +10493,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E3" s="15">
         <v>0</v>
@@ -11165,10 +11168,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>8</v>
@@ -11177,7 +11180,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F2" s="37">
         <v>0</v>
@@ -11185,10 +11188,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>8</v>
@@ -11197,7 +11200,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F3" s="37">
         <v>0</v>
@@ -11205,16 +11208,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C4" s="36" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>23</v>
@@ -11223,16 +11226,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E5" s="36" t="s">
         <v>23</v>
@@ -11243,16 +11246,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>23</v>
@@ -11263,16 +11266,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>23</v>
@@ -11281,16 +11284,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E8" s="36" t="s">
         <v>23</v>
@@ -11299,16 +11302,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>65</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>23</v>
@@ -11319,16 +11322,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="E10" s="36" t="s">
         <v>23</v>
@@ -11339,7 +11342,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>468</v>
@@ -11348,7 +11351,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="E11" s="36" t="s">
         <v>469</v>
@@ -11359,7 +11362,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>470</v>
@@ -11368,7 +11371,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="E12" s="36" t="s">
         <v>471</v>
@@ -11379,16 +11382,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E13" s="36" t="s">
         <v>23</v>
@@ -11397,16 +11400,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="35" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>23</v>
@@ -11425,9 +11428,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11440,22 +11443,22 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -11469,7 +11472,7 @@
       <c r="C2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="31" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -11489,7 +11492,7 @@
       <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -11507,7 +11510,7 @@
       <c r="C4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="31" t="s">
         <v>269</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -11525,7 +11528,7 @@
       <c r="C5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="31" t="s">
         <v>74</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -11545,7 +11548,7 @@
       <c r="C6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="31" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -11563,7 +11566,7 @@
       <c r="C7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="31" t="s">
         <v>166</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -11581,7 +11584,7 @@
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="17" t="s">
@@ -11601,7 +11604,7 @@
       <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="17" t="s">
@@ -11621,7 +11624,7 @@
       <c r="C10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="17" t="s">
@@ -11639,7 +11642,7 @@
       <c r="C11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="17" t="s">
@@ -11659,7 +11662,7 @@
       <c r="C12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="31" t="s">
         <v>579</v>
       </c>
       <c r="E12" s="17" t="s">
@@ -11677,7 +11680,7 @@
       <c r="C13" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="31" t="s">
         <v>581</v>
       </c>
       <c r="E13" s="17" t="s">
@@ -11695,7 +11698,7 @@
       <c r="C14" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="31" t="s">
         <v>583</v>
       </c>
       <c r="E14" s="17" t="s">
@@ -11715,7 +11718,7 @@
       <c r="C15" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="31" t="s">
         <v>585</v>
       </c>
       <c r="E15" s="17" t="s">
@@ -11733,8 +11736,8 @@
       <c r="C16" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>587</v>
+      <c r="D16" s="31" t="s">
+        <v>585</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>23</v>
@@ -11746,58 +11749,56 @@
         <v>574</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>589</v>
+      <c r="D17" s="31" t="s">
+        <v>588</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="18">
-        <v>0</v>
-      </c>
+      <c r="F17" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>591</v>
+      <c r="D18" s="31" t="s">
+        <v>590</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="18">
-        <v>27</v>
+      <c r="D19" s="31" t="s">
+        <v>592</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
+      <c r="F19" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="17" t="s">
@@ -11807,28 +11808,30 @@
         <v>593</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>378</v>
+        <v>65</v>
+      </c>
+      <c r="D20" s="18">
+        <v>27</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>162</v>
+        <v>594</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>379</v>
+      <c r="D21" s="31" t="s">
+        <v>378</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>23</v>
@@ -11840,13 +11843,13 @@
         <v>574</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>594</v>
+        <v>162</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>595</v>
+        <v>21</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>379</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>23</v>
@@ -11858,13 +11861,13 @@
         <v>574</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="31" t="s">
         <v>596</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>597</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>23</v>
@@ -11876,13 +11879,13 @@
         <v>574</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>381</v>
+        <v>597</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>382</v>
+      <c r="D24" s="31" t="s">
+        <v>598</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>23</v>
@@ -11894,16 +11897,16 @@
         <v>574</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>598</v>
+        <v>381</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>14</v>
+        <v>65</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>382</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="F25" s="16"/>
     </row>
@@ -11915,13 +11918,13 @@
         <v>599</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>600</v>
+        <v>8</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>14</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F26" s="16"/>
     </row>
@@ -11930,13 +11933,13 @@
         <v>574</v>
       </c>
       <c r="B27" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="31" t="s">
         <v>601</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>602</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>23</v>
@@ -11948,20 +11951,18 @@
         <v>574</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="31" t="s">
         <v>603</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>74</v>
-      </c>
       <c r="E28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="18">
-        <v>1</v>
-      </c>
+      <c r="F28" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="17" t="s">
@@ -11973,26 +11974,28 @@
       <c r="C29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>605</v>
+      <c r="D29" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="16"/>
+      <c r="F29" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="31" t="s">
         <v>606</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>607</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>23</v>
@@ -12004,13 +12007,13 @@
         <v>574</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>607</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="31" t="s">
         <v>608</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>609</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>23</v>
@@ -12022,13 +12025,13 @@
         <v>574</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="19" t="s">
-        <v>611</v>
+      <c r="D32" s="31" t="s">
+        <v>610</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>23</v>
@@ -12040,13 +12043,13 @@
         <v>574</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>613</v>
+      <c r="D33" s="31" t="s">
+        <v>612</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>23</v>
@@ -12058,13 +12061,13 @@
         <v>574</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>181</v>
+        <v>613</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>182</v>
+      <c r="D34" s="31" t="s">
+        <v>614</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>23</v>
@@ -12076,13 +12079,13 @@
         <v>574</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>614</v>
+        <v>181</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>615</v>
+      <c r="D35" s="31" t="s">
+        <v>182</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>23</v>
@@ -12094,13 +12097,13 @@
         <v>574</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>617</v>
+      <c r="D36" s="31" t="s">
+        <v>616</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>23</v>
@@ -12112,13 +12115,13 @@
         <v>574</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>617</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="31" t="s">
         <v>618</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>619</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>23</v>
@@ -12130,13 +12133,13 @@
         <v>574</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>619</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="31" t="s">
         <v>620</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>621</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>23</v>
@@ -12148,13 +12151,13 @@
         <v>574</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="31" t="s">
         <v>622</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>623</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>23</v>
@@ -12166,13 +12169,13 @@
         <v>574</v>
       </c>
       <c r="B40" s="17" t="s">
+        <v>623</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="31" t="s">
         <v>624</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>625</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>23</v>
@@ -12184,13 +12187,13 @@
         <v>574</v>
       </c>
       <c r="B41" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="31" t="s">
         <v>626</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>627</v>
       </c>
       <c r="E41" s="17" t="s">
         <v>23</v>
@@ -12202,13 +12205,13 @@
         <v>574</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="31" t="s">
         <v>628</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>629</v>
       </c>
       <c r="E42" s="17" t="s">
         <v>23</v>
@@ -12220,20 +12223,18 @@
         <v>574</v>
       </c>
       <c r="B43" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="31" t="s">
         <v>630</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>74</v>
-      </c>
       <c r="E43" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="18">
-        <v>1</v>
-      </c>
+      <c r="F43" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="17" t="s">
@@ -12245,67 +12246,69 @@
       <c r="C44" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="19" t="s">
-        <v>632</v>
+      <c r="D44" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="16"/>
+      <c r="F44" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B45" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="31" t="s">
         <v>633</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>634</v>
-      </c>
       <c r="E45" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F45" s="18">
-        <v>0</v>
-      </c>
+      <c r="F45" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B46" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="31" t="s">
         <v>635</v>
       </c>
-      <c r="C46" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>636</v>
-      </c>
       <c r="E46" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="F46" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+        <v>23</v>
+      </c>
+      <c r="F46" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B47" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="31" t="s">
         <v>637</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>638</v>
-      </c>
       <c r="E47" s="17" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="F47" s="16"/>
     </row>
@@ -12314,13 +12317,13 @@
         <v>574</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="31" t="s">
         <v>639</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>640</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>23</v>
@@ -12332,13 +12335,13 @@
         <v>574</v>
       </c>
       <c r="B49" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="31" t="s">
         <v>641</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>642</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>23</v>
@@ -12350,13 +12353,13 @@
         <v>574</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="19" t="s">
-        <v>644</v>
+      <c r="D50" s="31" t="s">
+        <v>643</v>
       </c>
       <c r="E50" s="17" t="s">
         <v>23</v>
@@ -12368,13 +12371,13 @@
         <v>574</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="19" t="s">
-        <v>642</v>
+      <c r="D51" s="31" t="s">
+        <v>645</v>
       </c>
       <c r="E51" s="17" t="s">
         <v>23</v>
@@ -12389,10 +12392,10 @@
         <v>646</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>648</v>
+        <v>65</v>
+      </c>
+      <c r="D52" s="31" t="s">
+        <v>643</v>
       </c>
       <c r="E52" s="17" t="s">
         <v>23</v>
@@ -12404,13 +12407,13 @@
         <v>574</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="D53" s="31" t="s">
         <v>649</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>650</v>
       </c>
       <c r="E53" s="17" t="s">
         <v>23</v>
@@ -12422,20 +12425,18 @@
         <v>574</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="19" t="s">
-        <v>650</v>
+      <c r="D54" s="31" t="s">
+        <v>651</v>
       </c>
       <c r="E54" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="18">
-        <v>1</v>
-      </c>
+      <c r="F54" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="17" t="s">
@@ -12447,13 +12448,15 @@
       <c r="C55" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="19" t="s">
-        <v>642</v>
+      <c r="D55" s="31" t="s">
+        <v>651</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="16"/>
+      <c r="F55" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="17" t="s">
@@ -12463,10 +12466,10 @@
         <v>653</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>654</v>
+        <v>65</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>643</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>23</v>
@@ -12478,128 +12481,146 @@
         <v>574</v>
       </c>
       <c r="B57" s="17" t="s">
+        <v>654</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="D57" s="31" t="s">
         <v>655</v>
       </c>
-      <c r="C57" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>14</v>
-      </c>
       <c r="E57" s="17" t="s">
-        <v>656</v>
-      </c>
-      <c r="F57" s="18">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F57" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B58" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="17" t="s">
         <v>657</v>
       </c>
-      <c r="C58" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>658</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F58" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="F58" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="17" t="s">
         <v>574</v>
       </c>
       <c r="B59" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="31" t="s">
         <v>659</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="E59" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="C60" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D59" s="19" t="s">
-        <v>660</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F59" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="30" t="s">
+      <c r="D60" s="31" t="s">
+        <v>661</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="B60" s="30" t="s">
-        <v>661</v>
-      </c>
-      <c r="C60" s="30" t="s">
+      <c r="B61" s="29" t="s">
+        <v>662</v>
+      </c>
+      <c r="C61" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>662</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F60" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="30" t="s">
+      <c r="D61" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="B61" s="30" t="s">
-        <v>663</v>
-      </c>
-      <c r="C61" s="30" t="s">
+      <c r="B62" s="29" t="s">
+        <v>664</v>
+      </c>
+      <c r="C62" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="E61" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F61" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="30" t="s">
+      <c r="D62" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="E62" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="B62" s="30" t="s">
-        <v>665</v>
-      </c>
-      <c r="C62" s="30" t="s">
+      <c r="B63" s="29" t="s">
+        <v>666</v>
+      </c>
+      <c r="C63" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="E62" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F62" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
-      <c r="A63" s="17" t="s">
+      <c r="D63" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F63" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+      <c r="A64" s="17" t="s">
         <v>574</v>
       </c>
-      <c r="B63" s="17" t="s">
-        <v>667</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="19" t="s">
+      <c r="B64" s="17" t="s">
         <v>668</v>
       </c>
-      <c r="E63" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F63" s="16"/>
+      <c r="C64" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>669</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13466,119 +13487,119 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>461</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>462</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>463</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>464</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>465</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="28" t="s">
+      <c r="C6" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>467</v>
       </c>
       <c r="F6" s="7">
@@ -13586,700 +13607,700 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="28" t="s">
+      <c r="C7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="28" t="s">
+      <c r="C8" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>468</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>469</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>470</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>471</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>472</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="26" t="s">
         <v>473</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="29">
+      <c r="E12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>474</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="28">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>475</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="28" t="s">
+      <c r="C14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="26" t="s">
         <v>476</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>477</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="28" t="s">
+      <c r="C15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>478</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="26" t="s">
         <v>476</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>479</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>480</v>
       </c>
-      <c r="E16" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="29">
+      <c r="E16" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>481</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="28" t="s">
+      <c r="C17" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="26" t="s">
         <v>476</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="30">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>482</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="26" t="s">
         <v>483</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>484</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="28" t="s">
+      <c r="C19" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="26" t="s">
         <v>486</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>487</v>
       </c>
-      <c r="E20" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="29">
+      <c r="E20" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>488</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="28" t="s">
+      <c r="C21" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>489</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="26" t="s">
         <v>490</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="28" t="s">
+      <c r="C22" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="26" t="s">
         <v>491</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>492</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>493</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>495</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="27">
         <v>27</v>
       </c>
-      <c r="E24" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="29">
+      <c r="E24" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="28">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>496</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="28" t="s">
+      <c r="C25" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>497</v>
       </c>
-      <c r="E25" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="29">
+      <c r="E25" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>498</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="28" t="s">
+      <c r="C26" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="26" t="s">
         <v>499</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="24" t="s">
         <v>460</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>500</v>
       </c>
-      <c r="C27" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="28" t="s">
+      <c r="C27" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>501</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="28">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>415</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="28" t="s">
+      <c r="C28" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="29"/>
+      <c r="E28" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>416</v>
       </c>
-      <c r="C29" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="28" t="s">
+      <c r="C29" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E29" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="29"/>
+      <c r="E29" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C30" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="28" t="s">
+      <c r="C30" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="E30" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="29"/>
+      <c r="E30" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="28" t="s">
+      <c r="C31" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="E31" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="29"/>
+      <c r="E31" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="C32" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="28" t="s">
+      <c r="C32" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="E32" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="29"/>
+      <c r="E32" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="28" t="s">
+      <c r="C33" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="27" t="s">
         <v>424</v>
       </c>
-      <c r="E33" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="29"/>
+      <c r="E33" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="C34" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="28" t="s">
+      <c r="C34" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="E34" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="29"/>
+      <c r="E34" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>429</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="27" t="s">
         <v>430</v>
       </c>
-      <c r="E35" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="29"/>
+      <c r="E35" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="27" t="s">
         <v>434</v>
       </c>
-      <c r="E36" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="29"/>
+      <c r="E36" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="26" t="s">
         <v>502</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="28" t="s">
+      <c r="C37" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="27" t="s">
         <v>503</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="26" t="s">
         <v>504</v>
       </c>
-      <c r="F37" s="31">
+      <c r="F37" s="30">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="26" t="s">
         <v>435</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="29"/>
+      <c r="E38" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="26" t="s">
         <v>436</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="27" t="s">
         <v>437</v>
       </c>
-      <c r="E39" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="31">
+      <c r="E39" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="30">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="26" t="s">
         <v>438</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="E40" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="31">
+      <c r="E40" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="30">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D41" s="27" t="s">
         <v>441</v>
       </c>
-      <c r="E41" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="29"/>
+      <c r="E41" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="28"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="27" t="s">
         <v>441</v>
       </c>
-      <c r="E42" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="29"/>
+      <c r="E42" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>